<commit_message>
Generate pdf files with all the groupings.
</commit_message>
<xml_diff>
--- a/sergei-walk-through/step4_community_detection_in_R/Communities-Unweighted.xlsx
+++ b/sergei-walk-through/step4_community_detection_in_R/Communities-Unweighted.xlsx
@@ -9,14 +9,23 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="17600" yWindow="6380" windowWidth="27820" windowHeight="17600" tabRatio="500"/>
+    <workbookView xWindow="8820" yWindow="3920" windowWidth="27820" windowHeight="17600" tabRatio="500" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="All Characters" sheetId="1" r:id="rId1"/>
-    <sheet name="Book1" sheetId="2" r:id="rId2"/>
+    <sheet name="Book1" sheetId="4" r:id="rId2"/>
+    <sheet name="Book2" sheetId="5" r:id="rId3"/>
+    <sheet name="Book3" sheetId="6" r:id="rId4"/>
+    <sheet name="Book4" sheetId="7" r:id="rId5"/>
+    <sheet name="Book5" sheetId="8" r:id="rId6"/>
   </sheets>
   <definedNames>
     <definedName name="all_NG_Nodes_1" localSheetId="0">'All Characters'!$A$1:$C$181</definedName>
+    <definedName name="book1_NG__Nodes" localSheetId="1">Book1!$B$1:$C$96</definedName>
+    <definedName name="book2_NG__Nodes" localSheetId="2">Book2!$B$1:$C$21</definedName>
+    <definedName name="book3_NG__Nodes" localSheetId="3">Book3!$B$1:$C$43</definedName>
+    <definedName name="book4_NG__Nodes" localSheetId="4">Book4!$B$1:$C$57</definedName>
+    <definedName name="book5_NG__Nodes" localSheetId="5">Book5!$B$1:$C$34</definedName>
   </definedNames>
   <calcPr calcId="150000" concurrentCalc="0"/>
   <extLst>
@@ -41,11 +50,56 @@
       </textFields>
     </textPr>
   </connection>
+  <connection id="2" name="book1-NG [Nodes]" type="6" refreshedVersion="0" background="1" saveData="1">
+    <textPr codePage="65001" sourceFile="/Applications/MAMP/htdocs/lesmiserables_DATA/sergei-walk-through/step4_community_detection_in_R/book1-NG [Nodes].csv" comma="1">
+      <textFields count="3">
+        <textField/>
+        <textField/>
+        <textField/>
+      </textFields>
+    </textPr>
+  </connection>
+  <connection id="3" name="book2-NG [Nodes]" type="6" refreshedVersion="0" background="1" saveData="1">
+    <textPr codePage="65001" sourceFile="/Applications/MAMP/htdocs/lesmiserables_DATA/sergei-walk-through/step4_community_detection_in_R/book2-NG [Nodes].csv" comma="1">
+      <textFields count="3">
+        <textField/>
+        <textField/>
+        <textField/>
+      </textFields>
+    </textPr>
+  </connection>
+  <connection id="4" name="book3-NG [Nodes]" type="6" refreshedVersion="0" background="1" saveData="1">
+    <textPr fileType="mac" codePage="65001" sourceFile="/Applications/MAMP/htdocs/lesmiserables_DATA/sergei-walk-through/step4_community_detection_in_R/book3-NG [Nodes].csv" comma="1">
+      <textFields count="3">
+        <textField/>
+        <textField/>
+        <textField/>
+      </textFields>
+    </textPr>
+  </connection>
+  <connection id="5" name="book4-NG [Nodes]" type="6" refreshedVersion="0" background="1" saveData="1">
+    <textPr codePage="65001" sourceFile="/Applications/MAMP/htdocs/lesmiserables_DATA/sergei-walk-through/step4_community_detection_in_R/book4-NG [Nodes].csv" comma="1">
+      <textFields count="3">
+        <textField/>
+        <textField/>
+        <textField/>
+      </textFields>
+    </textPr>
+  </connection>
+  <connection id="6" name="book5-NG [Nodes]" type="6" refreshedVersion="0" background="1" saveData="1">
+    <textPr codePage="65001" sourceFile="/Applications/MAMP/htdocs/lesmiserables_DATA/sergei-walk-through/step4_community_detection_in_R/book5-NG [Nodes].csv" comma="1">
+      <textFields count="3">
+        <textField/>
+        <textField/>
+        <textField/>
+      </textFields>
+    </textPr>
+  </connection>
 </connections>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="363" uniqueCount="363">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="870" uniqueCount="364">
   <si>
     <t>Name</t>
   </si>
@@ -1134,6 +1188,9 @@
   </si>
   <si>
     <t>Group</t>
+  </si>
+  <si>
+    <t>color</t>
   </si>
 </sst>
 </file>
@@ -1190,8 +1247,18 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="7">
+  <cellStyleXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1203,13 +1270,23 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="7">
+  <cellStyles count="17">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1224,6 +1301,26 @@
 
 <file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
 <queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="all-NG-Nodes_1" connectionId="1" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable2.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="book1-NG [Nodes]" connectionId="2" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable3.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="book2-NG [Nodes]" connectionId="3" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable4.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="book3-NG [Nodes]" connectionId="4" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable5.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="book4-NG [Nodes]" connectionId="5" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable6.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="book5-NG [Nodes]" connectionId="6" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1491,8 +1588,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C181"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3505,12 +3602,2880 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:C96"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD1048576"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="19.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="5.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6.33203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>20</v>
+      </c>
+      <c r="B3" t="s">
+        <v>21</v>
+      </c>
+      <c r="C3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>26</v>
+      </c>
+      <c r="B4" t="s">
+        <v>27</v>
+      </c>
+      <c r="C4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>22</v>
+      </c>
+      <c r="B5" t="s">
+        <v>23</v>
+      </c>
+      <c r="C5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>16</v>
+      </c>
+      <c r="B6" t="s">
+        <v>17</v>
+      </c>
+      <c r="C6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>30</v>
+      </c>
+      <c r="B7" t="s">
+        <v>31</v>
+      </c>
+      <c r="C7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>24</v>
+      </c>
+      <c r="B8" t="s">
+        <v>25</v>
+      </c>
+      <c r="C8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>18</v>
+      </c>
+      <c r="B9" t="s">
+        <v>19</v>
+      </c>
+      <c r="C9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>10</v>
+      </c>
+      <c r="B10" t="s">
+        <v>11</v>
+      </c>
+      <c r="C10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>14</v>
+      </c>
+      <c r="B11" t="s">
+        <v>15</v>
+      </c>
+      <c r="C11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>6</v>
+      </c>
+      <c r="B12" t="s">
+        <v>7</v>
+      </c>
+      <c r="C12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>12</v>
+      </c>
+      <c r="B13" t="s">
+        <v>13</v>
+      </c>
+      <c r="C13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>34</v>
+      </c>
+      <c r="B14" t="s">
+        <v>35</v>
+      </c>
+      <c r="C14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>8</v>
+      </c>
+      <c r="B15" t="s">
+        <v>9</v>
+      </c>
+      <c r="C15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>28</v>
+      </c>
+      <c r="B16" t="s">
+        <v>29</v>
+      </c>
+      <c r="C16">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>4</v>
+      </c>
+      <c r="B17" t="s">
+        <v>5</v>
+      </c>
+      <c r="C17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>32</v>
+      </c>
+      <c r="B18" t="s">
+        <v>33</v>
+      </c>
+      <c r="C18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>74</v>
+      </c>
+      <c r="B19" t="s">
+        <v>75</v>
+      </c>
+      <c r="C19">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>36</v>
+      </c>
+      <c r="B20" t="s">
+        <v>37</v>
+      </c>
+      <c r="C20">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>38</v>
+      </c>
+      <c r="B21" t="s">
+        <v>39</v>
+      </c>
+      <c r="C21">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>40</v>
+      </c>
+      <c r="B22" t="s">
+        <v>41</v>
+      </c>
+      <c r="C22">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>148</v>
+      </c>
+      <c r="B23" t="s">
+        <v>149</v>
+      </c>
+      <c r="C23">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>170</v>
+      </c>
+      <c r="B24" t="s">
+        <v>171</v>
+      </c>
+      <c r="C24">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>176</v>
+      </c>
+      <c r="B25" t="s">
+        <v>177</v>
+      </c>
+      <c r="C25">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>172</v>
+      </c>
+      <c r="B26" t="s">
+        <v>173</v>
+      </c>
+      <c r="C26">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>178</v>
+      </c>
+      <c r="B27" t="s">
+        <v>179</v>
+      </c>
+      <c r="C27">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>130</v>
+      </c>
+      <c r="B28" t="s">
+        <v>131</v>
+      </c>
+      <c r="C28">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
+        <v>174</v>
+      </c>
+      <c r="B29" t="s">
+        <v>175</v>
+      </c>
+      <c r="C29">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
+        <v>188</v>
+      </c>
+      <c r="B30" t="s">
+        <v>189</v>
+      </c>
+      <c r="C30">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
+        <v>182</v>
+      </c>
+      <c r="B31" t="s">
+        <v>183</v>
+      </c>
+      <c r="C31">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
+        <v>190</v>
+      </c>
+      <c r="B32" t="s">
+        <v>191</v>
+      </c>
+      <c r="C32">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A33" t="s">
+        <v>184</v>
+      </c>
+      <c r="B33" t="s">
+        <v>185</v>
+      </c>
+      <c r="C33">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A34" t="s">
+        <v>110</v>
+      </c>
+      <c r="B34" t="s">
+        <v>111</v>
+      </c>
+      <c r="C34">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A35" t="s">
+        <v>72</v>
+      </c>
+      <c r="B35" t="s">
+        <v>73</v>
+      </c>
+      <c r="C35">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A36" t="s">
+        <v>162</v>
+      </c>
+      <c r="B36" t="s">
+        <v>163</v>
+      </c>
+      <c r="C36">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A37" t="s">
+        <v>158</v>
+      </c>
+      <c r="B37" t="s">
+        <v>159</v>
+      </c>
+      <c r="C37">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A38" t="s">
+        <v>64</v>
+      </c>
+      <c r="B38" t="s">
+        <v>65</v>
+      </c>
+      <c r="C38">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A39" t="s">
+        <v>52</v>
+      </c>
+      <c r="B39" t="s">
+        <v>53</v>
+      </c>
+      <c r="C39">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A40" t="s">
+        <v>42</v>
+      </c>
+      <c r="B40" t="s">
+        <v>43</v>
+      </c>
+      <c r="C40">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A41" t="s">
+        <v>180</v>
+      </c>
+      <c r="B41" t="s">
+        <v>181</v>
+      </c>
+      <c r="C41">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A42" t="s">
+        <v>62</v>
+      </c>
+      <c r="B42" t="s">
+        <v>63</v>
+      </c>
+      <c r="C42">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A43" t="s">
+        <v>154</v>
+      </c>
+      <c r="B43" t="s">
+        <v>155</v>
+      </c>
+      <c r="C43">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A44" t="s">
+        <v>156</v>
+      </c>
+      <c r="B44" t="s">
+        <v>157</v>
+      </c>
+      <c r="C44">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A45" t="s">
+        <v>76</v>
+      </c>
+      <c r="B45" t="s">
+        <v>77</v>
+      </c>
+      <c r="C45">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A46" t="s">
+        <v>166</v>
+      </c>
+      <c r="B46" t="s">
+        <v>167</v>
+      </c>
+      <c r="C46">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A47" t="s">
+        <v>78</v>
+      </c>
+      <c r="B47" t="s">
+        <v>79</v>
+      </c>
+      <c r="C47">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A48" t="s">
+        <v>66</v>
+      </c>
+      <c r="B48" t="s">
+        <v>67</v>
+      </c>
+      <c r="C48">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A49" t="s">
+        <v>186</v>
+      </c>
+      <c r="B49" t="s">
+        <v>187</v>
+      </c>
+      <c r="C49">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A50" t="s">
+        <v>164</v>
+      </c>
+      <c r="B50" t="s">
+        <v>165</v>
+      </c>
+      <c r="C50">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A51" t="s">
+        <v>160</v>
+      </c>
+      <c r="B51" t="s">
+        <v>161</v>
+      </c>
+      <c r="C51">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A52" t="s">
+        <v>150</v>
+      </c>
+      <c r="B52" t="s">
+        <v>151</v>
+      </c>
+      <c r="C52">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A53" t="s">
+        <v>152</v>
+      </c>
+      <c r="B53" t="s">
+        <v>153</v>
+      </c>
+      <c r="C53">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A54" t="s">
+        <v>50</v>
+      </c>
+      <c r="B54" t="s">
+        <v>51</v>
+      </c>
+      <c r="C54">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A55" t="s">
+        <v>46</v>
+      </c>
+      <c r="B55" t="s">
+        <v>47</v>
+      </c>
+      <c r="C55">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A56" t="s">
+        <v>44</v>
+      </c>
+      <c r="B56" t="s">
+        <v>45</v>
+      </c>
+      <c r="C56">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A57" t="s">
+        <v>48</v>
+      </c>
+      <c r="B57" t="s">
+        <v>49</v>
+      </c>
+      <c r="C57">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A58" t="s">
+        <v>54</v>
+      </c>
+      <c r="B58" t="s">
+        <v>55</v>
+      </c>
+      <c r="C58">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A59" t="s">
+        <v>56</v>
+      </c>
+      <c r="B59" t="s">
+        <v>57</v>
+      </c>
+      <c r="C59">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A60" t="s">
+        <v>58</v>
+      </c>
+      <c r="B60" t="s">
+        <v>59</v>
+      </c>
+      <c r="C60">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A61" t="s">
+        <v>70</v>
+      </c>
+      <c r="B61" t="s">
+        <v>71</v>
+      </c>
+      <c r="C61">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A62" t="s">
+        <v>68</v>
+      </c>
+      <c r="B62" t="s">
+        <v>69</v>
+      </c>
+      <c r="C62">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A63" t="s">
+        <v>60</v>
+      </c>
+      <c r="B63" t="s">
+        <v>61</v>
+      </c>
+      <c r="C63">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A64" t="s">
+        <v>126</v>
+      </c>
+      <c r="B64" t="s">
+        <v>127</v>
+      </c>
+      <c r="C64">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A65" t="s">
+        <v>86</v>
+      </c>
+      <c r="B65" t="s">
+        <v>87</v>
+      </c>
+      <c r="C65">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A66" t="s">
+        <v>90</v>
+      </c>
+      <c r="B66" t="s">
+        <v>91</v>
+      </c>
+      <c r="C66">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A67" t="s">
+        <v>118</v>
+      </c>
+      <c r="B67" t="s">
+        <v>119</v>
+      </c>
+      <c r="C67">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A68" t="s">
+        <v>84</v>
+      </c>
+      <c r="B68" t="s">
+        <v>85</v>
+      </c>
+      <c r="C68">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A69" t="s">
+        <v>94</v>
+      </c>
+      <c r="B69" t="s">
+        <v>95</v>
+      </c>
+      <c r="C69">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A70" t="s">
+        <v>88</v>
+      </c>
+      <c r="B70" t="s">
+        <v>89</v>
+      </c>
+      <c r="C70">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A71" t="s">
+        <v>120</v>
+      </c>
+      <c r="B71" t="s">
+        <v>121</v>
+      </c>
+      <c r="C71">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A72" t="s">
+        <v>128</v>
+      </c>
+      <c r="B72" t="s">
+        <v>129</v>
+      </c>
+      <c r="C72">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="73" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A73" t="s">
+        <v>122</v>
+      </c>
+      <c r="B73" t="s">
+        <v>123</v>
+      </c>
+      <c r="C73">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="74" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A74" t="s">
+        <v>82</v>
+      </c>
+      <c r="B74" t="s">
+        <v>83</v>
+      </c>
+      <c r="C74">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="75" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A75" t="s">
+        <v>124</v>
+      </c>
+      <c r="B75" t="s">
+        <v>125</v>
+      </c>
+      <c r="C75">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="76" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A76" t="s">
+        <v>108</v>
+      </c>
+      <c r="B76" t="s">
+        <v>109</v>
+      </c>
+      <c r="C76">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="77" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A77" t="s">
+        <v>80</v>
+      </c>
+      <c r="B77" t="s">
+        <v>81</v>
+      </c>
+      <c r="C77">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="78" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A78" t="s">
+        <v>96</v>
+      </c>
+      <c r="B78" t="s">
+        <v>97</v>
+      </c>
+      <c r="C78">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="79" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A79" t="s">
+        <v>92</v>
+      </c>
+      <c r="B79" t="s">
+        <v>93</v>
+      </c>
+      <c r="C79">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="80" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A80" t="s">
+        <v>98</v>
+      </c>
+      <c r="B80" t="s">
+        <v>99</v>
+      </c>
+      <c r="C80">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="81" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A81" t="s">
+        <v>104</v>
+      </c>
+      <c r="B81" t="s">
+        <v>105</v>
+      </c>
+      <c r="C81">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="82" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A82" t="s">
+        <v>100</v>
+      </c>
+      <c r="B82" t="s">
+        <v>101</v>
+      </c>
+      <c r="C82">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="83" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A83" t="s">
+        <v>102</v>
+      </c>
+      <c r="B83" t="s">
+        <v>103</v>
+      </c>
+      <c r="C83">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="84" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A84" t="s">
+        <v>116</v>
+      </c>
+      <c r="B84" t="s">
+        <v>117</v>
+      </c>
+      <c r="C84">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="85" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A85" t="s">
+        <v>106</v>
+      </c>
+      <c r="B85" t="s">
+        <v>107</v>
+      </c>
+      <c r="C85">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="86" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A86" t="s">
+        <v>144</v>
+      </c>
+      <c r="B86" t="s">
+        <v>145</v>
+      </c>
+      <c r="C86">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="87" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A87" t="s">
+        <v>112</v>
+      </c>
+      <c r="B87" t="s">
+        <v>113</v>
+      </c>
+      <c r="C87">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="88" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A88" t="s">
+        <v>114</v>
+      </c>
+      <c r="B88" t="s">
+        <v>115</v>
+      </c>
+      <c r="C88">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="89" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A89" t="s">
+        <v>132</v>
+      </c>
+      <c r="B89" t="s">
+        <v>133</v>
+      </c>
+      <c r="C89">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="90" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A90" t="s">
+        <v>146</v>
+      </c>
+      <c r="B90" t="s">
+        <v>147</v>
+      </c>
+      <c r="C90">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="91" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A91" t="s">
+        <v>134</v>
+      </c>
+      <c r="B91" t="s">
+        <v>135</v>
+      </c>
+      <c r="C91">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="92" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A92" t="s">
+        <v>168</v>
+      </c>
+      <c r="B92" t="s">
+        <v>169</v>
+      </c>
+      <c r="C92">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="93" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A93" t="s">
+        <v>136</v>
+      </c>
+      <c r="B93" t="s">
+        <v>137</v>
+      </c>
+      <c r="C93">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="94" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A94" t="s">
+        <v>138</v>
+      </c>
+      <c r="B94" t="s">
+        <v>139</v>
+      </c>
+      <c r="C94">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="95" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A95" t="s">
+        <v>140</v>
+      </c>
+      <c r="B95" t="s">
+        <v>141</v>
+      </c>
+      <c r="C95">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="96" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A96" t="s">
+        <v>142</v>
+      </c>
+      <c r="B96" t="s">
+        <v>143</v>
+      </c>
+      <c r="C96">
+        <v>13</v>
+      </c>
+    </row>
+  </sheetData>
+  <sortState ref="A2:D96">
+    <sortCondition ref="C2:C96"/>
+    <sortCondition ref="A2:A96"/>
+  </sortState>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C21"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="21.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="5.1640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>363</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>196</v>
+      </c>
+      <c r="B2" t="s">
+        <v>197</v>
+      </c>
+      <c r="C2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>194</v>
+      </c>
+      <c r="B3" t="s">
+        <v>195</v>
+      </c>
+      <c r="C3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>106</v>
+      </c>
+      <c r="B4" t="s">
+        <v>107</v>
+      </c>
+      <c r="C4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>198</v>
+      </c>
+      <c r="B5" t="s">
+        <v>199</v>
+      </c>
+      <c r="C5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>206</v>
+      </c>
+      <c r="B6" t="s">
+        <v>207</v>
+      </c>
+      <c r="C6">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>114</v>
+      </c>
+      <c r="B7" t="s">
+        <v>115</v>
+      </c>
+      <c r="C7">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>42</v>
+      </c>
+      <c r="B8" t="s">
+        <v>43</v>
+      </c>
+      <c r="C8">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>210</v>
+      </c>
+      <c r="B9" t="s">
+        <v>211</v>
+      </c>
+      <c r="C9">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>204</v>
+      </c>
+      <c r="B10" t="s">
+        <v>205</v>
+      </c>
+      <c r="C10">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>208</v>
+      </c>
+      <c r="B11" t="s">
+        <v>209</v>
+      </c>
+      <c r="C11">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>214</v>
+      </c>
+      <c r="B12" t="s">
+        <v>215</v>
+      </c>
+      <c r="C12">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>212</v>
+      </c>
+      <c r="B13" t="s">
+        <v>213</v>
+      </c>
+      <c r="C13">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>98</v>
+      </c>
+      <c r="B14" t="s">
+        <v>99</v>
+      </c>
+      <c r="C14">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>104</v>
+      </c>
+      <c r="B15" t="s">
+        <v>105</v>
+      </c>
+      <c r="C15">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>100</v>
+      </c>
+      <c r="B16" t="s">
+        <v>101</v>
+      </c>
+      <c r="C16">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>200</v>
+      </c>
+      <c r="B17" t="s">
+        <v>201</v>
+      </c>
+      <c r="C17">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>102</v>
+      </c>
+      <c r="B18" t="s">
+        <v>103</v>
+      </c>
+      <c r="C18">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>202</v>
+      </c>
+      <c r="B19" t="s">
+        <v>203</v>
+      </c>
+      <c r="C19">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>112</v>
+      </c>
+      <c r="B20" t="s">
+        <v>113</v>
+      </c>
+      <c r="C20">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>216</v>
+      </c>
+      <c r="B21" t="s">
+        <v>217</v>
+      </c>
+      <c r="C21">
+        <v>4</v>
+      </c>
+    </row>
+  </sheetData>
+  <sortState ref="B2:D21">
+    <sortCondition ref="C2:C21"/>
+  </sortState>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C43"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="17.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="5.1640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>363</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>98</v>
+      </c>
+      <c r="B2" t="s">
+        <v>99</v>
+      </c>
+      <c r="C2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>280</v>
+      </c>
+      <c r="B3" t="s">
+        <v>281</v>
+      </c>
+      <c r="C3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>196</v>
+      </c>
+      <c r="B4" t="s">
+        <v>197</v>
+      </c>
+      <c r="C4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>276</v>
+      </c>
+      <c r="B5" t="s">
+        <v>277</v>
+      </c>
+      <c r="C5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>270</v>
+      </c>
+      <c r="B6" t="s">
+        <v>271</v>
+      </c>
+      <c r="C6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>104</v>
+      </c>
+      <c r="B7" t="s">
+        <v>105</v>
+      </c>
+      <c r="C7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>278</v>
+      </c>
+      <c r="B8" t="s">
+        <v>279</v>
+      </c>
+      <c r="C8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>100</v>
+      </c>
+      <c r="B9" t="s">
+        <v>101</v>
+      </c>
+      <c r="C9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>268</v>
+      </c>
+      <c r="B10" t="s">
+        <v>269</v>
+      </c>
+      <c r="C10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>114</v>
+      </c>
+      <c r="B11" t="s">
+        <v>115</v>
+      </c>
+      <c r="C11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>42</v>
+      </c>
+      <c r="B12" t="s">
+        <v>43</v>
+      </c>
+      <c r="C12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>228</v>
+      </c>
+      <c r="B13" t="s">
+        <v>229</v>
+      </c>
+      <c r="C13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>260</v>
+      </c>
+      <c r="B14" t="s">
+        <v>261</v>
+      </c>
+      <c r="C14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>102</v>
+      </c>
+      <c r="B15" t="s">
+        <v>103</v>
+      </c>
+      <c r="C15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>274</v>
+      </c>
+      <c r="B16" t="s">
+        <v>275</v>
+      </c>
+      <c r="C16">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>272</v>
+      </c>
+      <c r="B17" t="s">
+        <v>273</v>
+      </c>
+      <c r="C17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>266</v>
+      </c>
+      <c r="B18" t="s">
+        <v>267</v>
+      </c>
+      <c r="C18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>106</v>
+      </c>
+      <c r="B19" t="s">
+        <v>107</v>
+      </c>
+      <c r="C19">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>230</v>
+      </c>
+      <c r="B20" t="s">
+        <v>231</v>
+      </c>
+      <c r="C20">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>232</v>
+      </c>
+      <c r="B21" t="s">
+        <v>233</v>
+      </c>
+      <c r="C21">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>220</v>
+      </c>
+      <c r="B22" t="s">
+        <v>221</v>
+      </c>
+      <c r="C22">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>222</v>
+      </c>
+      <c r="B23" t="s">
+        <v>223</v>
+      </c>
+      <c r="C23">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>12</v>
+      </c>
+      <c r="B24" t="s">
+        <v>13</v>
+      </c>
+      <c r="C24">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>224</v>
+      </c>
+      <c r="B25" t="s">
+        <v>225</v>
+      </c>
+      <c r="C25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>226</v>
+      </c>
+      <c r="B26" t="s">
+        <v>227</v>
+      </c>
+      <c r="C26">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>236</v>
+      </c>
+      <c r="B27" t="s">
+        <v>237</v>
+      </c>
+      <c r="C27">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>194</v>
+      </c>
+      <c r="B28" t="s">
+        <v>195</v>
+      </c>
+      <c r="C28">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
+        <v>242</v>
+      </c>
+      <c r="B29" t="s">
+        <v>243</v>
+      </c>
+      <c r="C29">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
+        <v>240</v>
+      </c>
+      <c r="B30" t="s">
+        <v>241</v>
+      </c>
+      <c r="C30">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
+        <v>238</v>
+      </c>
+      <c r="B31" t="s">
+        <v>239</v>
+      </c>
+      <c r="C31">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
+        <v>258</v>
+      </c>
+      <c r="B32" t="s">
+        <v>259</v>
+      </c>
+      <c r="C32">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A33" t="s">
+        <v>4</v>
+      </c>
+      <c r="B33" t="s">
+        <v>5</v>
+      </c>
+      <c r="C33">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A34" t="s">
+        <v>234</v>
+      </c>
+      <c r="B34" t="s">
+        <v>235</v>
+      </c>
+      <c r="C34">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A35" t="s">
+        <v>248</v>
+      </c>
+      <c r="B35" t="s">
+        <v>249</v>
+      </c>
+      <c r="C35">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A36" t="s">
+        <v>244</v>
+      </c>
+      <c r="B36" t="s">
+        <v>245</v>
+      </c>
+      <c r="C36">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A37" t="s">
+        <v>250</v>
+      </c>
+      <c r="B37" t="s">
+        <v>251</v>
+      </c>
+      <c r="C37">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A38" t="s">
+        <v>246</v>
+      </c>
+      <c r="B38" t="s">
+        <v>247</v>
+      </c>
+      <c r="C38">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A39" t="s">
+        <v>252</v>
+      </c>
+      <c r="B39" t="s">
+        <v>253</v>
+      </c>
+      <c r="C39">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A40" t="s">
+        <v>254</v>
+      </c>
+      <c r="B40" t="s">
+        <v>255</v>
+      </c>
+      <c r="C40">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A41" t="s">
+        <v>256</v>
+      </c>
+      <c r="B41" t="s">
+        <v>257</v>
+      </c>
+      <c r="C41">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A42" t="s">
+        <v>264</v>
+      </c>
+      <c r="B42" t="s">
+        <v>265</v>
+      </c>
+      <c r="C42">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A43" t="s">
+        <v>262</v>
+      </c>
+      <c r="B43" t="s">
+        <v>263</v>
+      </c>
+      <c r="C43">
+        <v>5</v>
+      </c>
+    </row>
+  </sheetData>
+  <sortState ref="A2:D43">
+    <sortCondition ref="C2:C43"/>
+    <sortCondition ref="A2:A43"/>
+  </sortState>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C57"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="19.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="5.1640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>363</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>248</v>
+      </c>
+      <c r="B2" t="s">
+        <v>249</v>
+      </c>
+      <c r="C2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>244</v>
+      </c>
+      <c r="B3" t="s">
+        <v>245</v>
+      </c>
+      <c r="C3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>284</v>
+      </c>
+      <c r="B4" t="s">
+        <v>285</v>
+      </c>
+      <c r="C4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>250</v>
+      </c>
+      <c r="B5" t="s">
+        <v>251</v>
+      </c>
+      <c r="C5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>320</v>
+      </c>
+      <c r="B6" t="s">
+        <v>321</v>
+      </c>
+      <c r="C6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>104</v>
+      </c>
+      <c r="B7" t="s">
+        <v>105</v>
+      </c>
+      <c r="C7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>246</v>
+      </c>
+      <c r="B8" t="s">
+        <v>247</v>
+      </c>
+      <c r="C8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>330</v>
+      </c>
+      <c r="B9" t="s">
+        <v>331</v>
+      </c>
+      <c r="C9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>336</v>
+      </c>
+      <c r="B10" t="s">
+        <v>337</v>
+      </c>
+      <c r="C10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>252</v>
+      </c>
+      <c r="B11" t="s">
+        <v>253</v>
+      </c>
+      <c r="C11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>282</v>
+      </c>
+      <c r="B12" t="s">
+        <v>283</v>
+      </c>
+      <c r="C12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>310</v>
+      </c>
+      <c r="B13" t="s">
+        <v>311</v>
+      </c>
+      <c r="C13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>200</v>
+      </c>
+      <c r="B14" t="s">
+        <v>201</v>
+      </c>
+      <c r="C14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>326</v>
+      </c>
+      <c r="B15" t="s">
+        <v>327</v>
+      </c>
+      <c r="C15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>334</v>
+      </c>
+      <c r="B16" t="s">
+        <v>335</v>
+      </c>
+      <c r="C16">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>254</v>
+      </c>
+      <c r="B17" t="s">
+        <v>255</v>
+      </c>
+      <c r="C17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>114</v>
+      </c>
+      <c r="B18" t="s">
+        <v>115</v>
+      </c>
+      <c r="C18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>256</v>
+      </c>
+      <c r="B19" t="s">
+        <v>257</v>
+      </c>
+      <c r="C19">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>240</v>
+      </c>
+      <c r="B20" t="s">
+        <v>241</v>
+      </c>
+      <c r="C20">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>228</v>
+      </c>
+      <c r="B21" t="s">
+        <v>229</v>
+      </c>
+      <c r="C21">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>324</v>
+      </c>
+      <c r="B22" t="s">
+        <v>325</v>
+      </c>
+      <c r="C22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>262</v>
+      </c>
+      <c r="B23" t="s">
+        <v>263</v>
+      </c>
+      <c r="C23">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>322</v>
+      </c>
+      <c r="B24" t="s">
+        <v>323</v>
+      </c>
+      <c r="C24">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>258</v>
+      </c>
+      <c r="B25" t="s">
+        <v>259</v>
+      </c>
+      <c r="C25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>328</v>
+      </c>
+      <c r="B26" t="s">
+        <v>329</v>
+      </c>
+      <c r="C26">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>302</v>
+      </c>
+      <c r="B27" t="s">
+        <v>303</v>
+      </c>
+      <c r="C27">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>300</v>
+      </c>
+      <c r="B28" t="s">
+        <v>301</v>
+      </c>
+      <c r="C28">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
+        <v>264</v>
+      </c>
+      <c r="B29" t="s">
+        <v>265</v>
+      </c>
+      <c r="C29">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
+        <v>314</v>
+      </c>
+      <c r="B30" t="s">
+        <v>315</v>
+      </c>
+      <c r="C30">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
+        <v>312</v>
+      </c>
+      <c r="B31" t="s">
+        <v>313</v>
+      </c>
+      <c r="C31">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
+        <v>226</v>
+      </c>
+      <c r="B32" t="s">
+        <v>227</v>
+      </c>
+      <c r="C32">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A33" t="s">
+        <v>316</v>
+      </c>
+      <c r="B33" t="s">
+        <v>317</v>
+      </c>
+      <c r="C33">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A34" t="s">
+        <v>290</v>
+      </c>
+      <c r="B34" t="s">
+        <v>291</v>
+      </c>
+      <c r="C34">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A35" t="s">
+        <v>280</v>
+      </c>
+      <c r="B35" t="s">
+        <v>281</v>
+      </c>
+      <c r="C35">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A36" t="s">
+        <v>276</v>
+      </c>
+      <c r="B36" t="s">
+        <v>277</v>
+      </c>
+      <c r="C36">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A37" t="s">
+        <v>270</v>
+      </c>
+      <c r="B37" t="s">
+        <v>271</v>
+      </c>
+      <c r="C37">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A38" t="s">
+        <v>100</v>
+      </c>
+      <c r="B38" t="s">
+        <v>101</v>
+      </c>
+      <c r="C38">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A39" t="s">
+        <v>286</v>
+      </c>
+      <c r="B39" t="s">
+        <v>287</v>
+      </c>
+      <c r="C39">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A40" t="s">
+        <v>268</v>
+      </c>
+      <c r="B40" t="s">
+        <v>269</v>
+      </c>
+      <c r="C40">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A41" t="s">
+        <v>42</v>
+      </c>
+      <c r="B41" t="s">
+        <v>43</v>
+      </c>
+      <c r="C41">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A42" t="s">
+        <v>292</v>
+      </c>
+      <c r="B42" t="s">
+        <v>293</v>
+      </c>
+      <c r="C42">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A43" t="s">
+        <v>332</v>
+      </c>
+      <c r="B43" t="s">
+        <v>333</v>
+      </c>
+      <c r="C43">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A44" t="s">
+        <v>266</v>
+      </c>
+      <c r="B44" t="s">
+        <v>267</v>
+      </c>
+      <c r="C44">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A45" t="s">
+        <v>106</v>
+      </c>
+      <c r="B45" t="s">
+        <v>107</v>
+      </c>
+      <c r="C45">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A46" t="s">
+        <v>288</v>
+      </c>
+      <c r="B46" t="s">
+        <v>289</v>
+      </c>
+      <c r="C46">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A47" t="s">
+        <v>304</v>
+      </c>
+      <c r="B47" t="s">
+        <v>305</v>
+      </c>
+      <c r="C47">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A48" t="s">
+        <v>220</v>
+      </c>
+      <c r="B48" t="s">
+        <v>221</v>
+      </c>
+      <c r="C48">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A49" t="s">
+        <v>222</v>
+      </c>
+      <c r="B49" t="s">
+        <v>223</v>
+      </c>
+      <c r="C49">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A50" t="s">
+        <v>12</v>
+      </c>
+      <c r="B50" t="s">
+        <v>13</v>
+      </c>
+      <c r="C50">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A51" t="s">
+        <v>102</v>
+      </c>
+      <c r="B51" t="s">
+        <v>103</v>
+      </c>
+      <c r="C51">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A52" t="s">
+        <v>318</v>
+      </c>
+      <c r="B52" t="s">
+        <v>319</v>
+      </c>
+      <c r="C52">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A53" t="s">
+        <v>294</v>
+      </c>
+      <c r="B53" t="s">
+        <v>295</v>
+      </c>
+      <c r="C53">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A54" t="s">
+        <v>298</v>
+      </c>
+      <c r="B54" t="s">
+        <v>299</v>
+      </c>
+      <c r="C54">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A55" t="s">
+        <v>296</v>
+      </c>
+      <c r="B55" t="s">
+        <v>297</v>
+      </c>
+      <c r="C55">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A56" t="s">
+        <v>306</v>
+      </c>
+      <c r="B56" t="s">
+        <v>307</v>
+      </c>
+      <c r="C56">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A57" t="s">
+        <v>308</v>
+      </c>
+      <c r="B57" t="s">
+        <v>309</v>
+      </c>
+      <c r="C57">
+        <v>4</v>
+      </c>
+    </row>
+  </sheetData>
+  <sortState ref="A2:D57">
+    <sortCondition ref="C2:C57"/>
+    <sortCondition ref="A2:A57"/>
+  </sortState>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C34"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:XFD1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="22.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="5.1640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>363</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>244</v>
+      </c>
+      <c r="B2" t="s">
+        <v>245</v>
+      </c>
+      <c r="C2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>250</v>
+      </c>
+      <c r="B3" t="s">
+        <v>251</v>
+      </c>
+      <c r="C3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>246</v>
+      </c>
+      <c r="B4" t="s">
+        <v>247</v>
+      </c>
+      <c r="C4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>252</v>
+      </c>
+      <c r="B5" t="s">
+        <v>253</v>
+      </c>
+      <c r="C5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>282</v>
+      </c>
+      <c r="B6" t="s">
+        <v>283</v>
+      </c>
+      <c r="C6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>200</v>
+      </c>
+      <c r="B7" t="s">
+        <v>201</v>
+      </c>
+      <c r="C7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>334</v>
+      </c>
+      <c r="B8" t="s">
+        <v>335</v>
+      </c>
+      <c r="C8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>254</v>
+      </c>
+      <c r="B9" t="s">
+        <v>255</v>
+      </c>
+      <c r="C9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>340</v>
+      </c>
+      <c r="B10" t="s">
+        <v>341</v>
+      </c>
+      <c r="C10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>114</v>
+      </c>
+      <c r="B11" t="s">
+        <v>115</v>
+      </c>
+      <c r="C11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>350</v>
+      </c>
+      <c r="B12" t="s">
+        <v>351</v>
+      </c>
+      <c r="C12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>42</v>
+      </c>
+      <c r="B13" t="s">
+        <v>43</v>
+      </c>
+      <c r="C13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>256</v>
+      </c>
+      <c r="B14" t="s">
+        <v>257</v>
+      </c>
+      <c r="C14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>228</v>
+      </c>
+      <c r="B15" t="s">
+        <v>229</v>
+      </c>
+      <c r="C15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>348</v>
+      </c>
+      <c r="B16" t="s">
+        <v>349</v>
+      </c>
+      <c r="C16">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>342</v>
+      </c>
+      <c r="B17" t="s">
+        <v>343</v>
+      </c>
+      <c r="C17">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>344</v>
+      </c>
+      <c r="B18" t="s">
+        <v>345</v>
+      </c>
+      <c r="C18">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>346</v>
+      </c>
+      <c r="B19" t="s">
+        <v>347</v>
+      </c>
+      <c r="C19">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>294</v>
+      </c>
+      <c r="B20" t="s">
+        <v>295</v>
+      </c>
+      <c r="C20">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>296</v>
+      </c>
+      <c r="B21" t="s">
+        <v>297</v>
+      </c>
+      <c r="C21">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>100</v>
+      </c>
+      <c r="B22" t="s">
+        <v>101</v>
+      </c>
+      <c r="C22">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>98</v>
+      </c>
+      <c r="B23" t="s">
+        <v>99</v>
+      </c>
+      <c r="C23">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>106</v>
+      </c>
+      <c r="B24" t="s">
+        <v>107</v>
+      </c>
+      <c r="C24">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>304</v>
+      </c>
+      <c r="B25" t="s">
+        <v>305</v>
+      </c>
+      <c r="C25">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>352</v>
+      </c>
+      <c r="B26" t="s">
+        <v>353</v>
+      </c>
+      <c r="C26">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>104</v>
+      </c>
+      <c r="B27" t="s">
+        <v>105</v>
+      </c>
+      <c r="C27">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>356</v>
+      </c>
+      <c r="B28" t="s">
+        <v>357</v>
+      </c>
+      <c r="C28">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
+        <v>220</v>
+      </c>
+      <c r="B29" t="s">
+        <v>221</v>
+      </c>
+      <c r="C29">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
+        <v>12</v>
+      </c>
+      <c r="B30" t="s">
+        <v>13</v>
+      </c>
+      <c r="C30">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
+        <v>354</v>
+      </c>
+      <c r="B31" t="s">
+        <v>355</v>
+      </c>
+      <c r="C31">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
+        <v>196</v>
+      </c>
+      <c r="B32" t="s">
+        <v>197</v>
+      </c>
+      <c r="C32">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A33" t="s">
+        <v>358</v>
+      </c>
+      <c r="B33" t="s">
+        <v>359</v>
+      </c>
+      <c r="C33">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A34" t="s">
+        <v>360</v>
+      </c>
+      <c r="B34" t="s">
+        <v>361</v>
+      </c>
+      <c r="C34">
+        <v>8</v>
+      </c>
+    </row>
+  </sheetData>
+  <sortState ref="A2:D34">
+    <sortCondition ref="C2:C34"/>
+    <sortCondition ref="A2:A34"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>